<commit_message>
Working code with full functionality except load/store graphs
</commit_message>
<xml_diff>
--- a/Logs/check_code/training_episode_output.xlsx
+++ b/Logs/check_code/training_episode_output.xlsx
@@ -408,27 +408,27 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2">
-        <v>-9.72700023651123</v>
+        <v>-9.729999542236328</v>
       </c>
       <c r="B2">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C2">
-        <v>8.927000045776367</v>
+        <v>8.529999732971191</v>
       </c>
       <c r="D2">
-        <v>12.15875053405762</v>
+        <v>8.108332633972168</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3">
-        <v>-11.99199962615967</v>
+        <v>-11.98999977111816</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
       <c r="C3">
-        <v>11.99199962615967</v>
+        <v>11.98999977111816</v>
       </c>
       <c r="D3" t="s">
         <v>4</v>
@@ -436,13 +436,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4">
-        <v>-9.694999694824219</v>
+        <v>-9.699999809265137</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
       <c r="C4">
-        <v>9.694999694824219</v>
+        <v>9.699999809265137</v>
       </c>
       <c r="D4" t="s">
         <v>4</v>
@@ -450,13 +450,13 @@
     </row>
     <row r="5" spans="1:4">
       <c r="A5">
-        <v>-2.437999963760376</v>
+        <v>-2.440000057220459</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>2.437999963760376</v>
+        <v>2.440000057220459</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -464,44 +464,44 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6">
-        <v>-2.427999973297119</v>
+        <v>-2.430000066757202</v>
       </c>
       <c r="B6">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C6">
-        <v>1.628000020980835</v>
+        <v>1.230000019073486</v>
       </c>
       <c r="D6">
-        <v>3.034999847412109</v>
+        <v>2.024999856948853</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7">
-        <v>-4.632999897003174</v>
+        <v>-4.630000114440918</v>
       </c>
       <c r="B7">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C7">
-        <v>3.83299994468689</v>
+        <v>3.430000066757202</v>
       </c>
       <c r="D7">
-        <v>5.791249752044678</v>
+        <v>3.858333349227905</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8">
-        <v>-7.026999950408936</v>
+        <v>-7.03000020980835</v>
       </c>
       <c r="B8">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C8">
-        <v>6.226999759674072</v>
+        <v>5.829999923706055</v>
       </c>
       <c r="D8">
-        <v>8.783749580383301</v>
+        <v>5.858333110809326</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -520,27 +520,27 @@
     </row>
     <row r="10" spans="1:4">
       <c r="A10">
-        <v>-14.78899955749512</v>
+        <v>-14.78999996185303</v>
       </c>
       <c r="B10">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C10">
-        <v>13.98899936676025</v>
+        <v>13.59000015258789</v>
       </c>
       <c r="D10">
-        <v>18.48624992370605</v>
+        <v>12.32499980926514</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11">
-        <v>-14.54699993133545</v>
+        <v>-14.55000019073486</v>
       </c>
       <c r="B11">
         <v>0</v>
       </c>
       <c r="C11">
-        <v>14.54699993133545</v>
+        <v>14.55000019073486</v>
       </c>
       <c r="D11" t="s">
         <v>4</v>
@@ -548,13 +548,13 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12">
-        <v>-13.8120002746582</v>
+        <v>-13.8100004196167</v>
       </c>
       <c r="B12">
         <v>0</v>
       </c>
       <c r="C12">
-        <v>13.8120002746582</v>
+        <v>13.8100004196167</v>
       </c>
       <c r="D12" t="s">
         <v>4</v>
@@ -562,13 +562,13 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13">
-        <v>-9.843999862670898</v>
+        <v>-9.840000152587891</v>
       </c>
       <c r="B13">
         <v>0</v>
       </c>
       <c r="C13">
-        <v>9.843999862670898</v>
+        <v>9.840000152587891</v>
       </c>
       <c r="D13" t="s">
         <v>4</v>
@@ -576,13 +576,13 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14">
-        <v>-9.921999931335449</v>
+        <v>-9.920000076293945</v>
       </c>
       <c r="B14">
         <v>0</v>
       </c>
       <c r="C14">
-        <v>9.921999931335449</v>
+        <v>9.920000076293945</v>
       </c>
       <c r="D14" t="s">
         <v>4</v>
@@ -590,13 +590,13 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15">
-        <v>-8.031000137329102</v>
+        <v>-8.029999732971191</v>
       </c>
       <c r="B15">
         <v>0</v>
       </c>
       <c r="C15">
-        <v>8.031000137329102</v>
+        <v>8.029999732971191</v>
       </c>
       <c r="D15" t="s">
         <v>4</v>
@@ -604,27 +604,27 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16">
-        <v>-7.617000102996826</v>
+        <v>-7.619999885559082</v>
       </c>
       <c r="B16">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C16">
-        <v>6.816999912261963</v>
+        <v>6.420000076293945</v>
       </c>
       <c r="D16">
-        <v>9.521249771118164</v>
+        <v>6.34999942779541</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17">
-        <v>-10.36699962615967</v>
+        <v>-10.36999988555908</v>
       </c>
       <c r="B17">
         <v>0</v>
       </c>
       <c r="C17">
-        <v>10.36699962615967</v>
+        <v>10.36999988555908</v>
       </c>
       <c r="D17" t="s">
         <v>4</v>
@@ -632,13 +632,13 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18">
-        <v>-14.30500030517578</v>
+        <v>-14.30000019073486</v>
       </c>
       <c r="B18">
         <v>0</v>
       </c>
       <c r="C18">
-        <v>14.30500030517578</v>
+        <v>14.30000019073486</v>
       </c>
       <c r="D18" t="s">
         <v>4</v>
@@ -646,13 +646,13 @@
     </row>
     <row r="19" spans="1:4">
       <c r="A19">
-        <v>-11.24199962615967</v>
+        <v>-11.23999977111816</v>
       </c>
       <c r="B19">
         <v>0</v>
       </c>
       <c r="C19">
-        <v>11.24199962615967</v>
+        <v>11.23999977111816</v>
       </c>
       <c r="D19" t="s">
         <v>4</v>
@@ -660,13 +660,13 @@
     </row>
     <row r="20" spans="1:4">
       <c r="A20">
-        <v>-3.351999998092651</v>
+        <v>-3.349999904632568</v>
       </c>
       <c r="B20">
         <v>0</v>
       </c>
       <c r="C20">
-        <v>3.351999998092651</v>
+        <v>3.349999904632568</v>
       </c>
       <c r="D20" t="s">
         <v>4</v>
@@ -674,27 +674,27 @@
     </row>
     <row r="21" spans="1:4">
       <c r="A21">
-        <v>-13.97700023651123</v>
+        <v>-13.97999954223633</v>
       </c>
       <c r="B21">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C21">
-        <v>13.17700004577637</v>
+        <v>12.77999973297119</v>
       </c>
       <c r="D21">
-        <v>17.47125053405762</v>
+        <v>11.64999961853027</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22">
-        <v>-4.757999897003174</v>
+        <v>-4.760000228881836</v>
       </c>
       <c r="B22">
         <v>0</v>
       </c>
       <c r="C22">
-        <v>4.757999897003174</v>
+        <v>4.760000228881836</v>
       </c>
       <c r="D22" t="s">
         <v>4</v>
@@ -702,16 +702,16 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23">
-        <v>-1.835000038146973</v>
+        <v>-1.830000042915344</v>
       </c>
       <c r="B23">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C23">
-        <v>1.035000085830688</v>
+        <v>0.6299999952316284</v>
       </c>
       <c r="D23">
-        <v>2.293750047683716</v>
+        <v>1.524999976158142</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -719,38 +719,38 @@
         <v>-2.269999980926514</v>
       </c>
       <c r="B24">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C24">
-        <v>1.470000028610229</v>
+        <v>1.069999933242798</v>
       </c>
       <c r="D24">
-        <v>2.837499856948853</v>
+        <v>1.891666531562805</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25">
-        <v>-12.51599979400635</v>
+        <v>-12.52000045776367</v>
       </c>
       <c r="B25">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C25">
-        <v>11.71599960327148</v>
+        <v>11.32000064849854</v>
       </c>
       <c r="D25">
-        <v>15.64499950408936</v>
+        <v>10.43333339691162</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26">
-        <v>-2.818000078201294</v>
+        <v>-2.819999933242798</v>
       </c>
       <c r="B26">
         <v>0</v>
       </c>
       <c r="C26">
-        <v>2.818000078201294</v>
+        <v>2.819999933242798</v>
       </c>
       <c r="D26" t="s">
         <v>4</v>
@@ -758,16 +758,16 @@
     </row>
     <row r="27" spans="1:4">
       <c r="A27">
-        <v>-6.418000221252441</v>
+        <v>-6.420000076293945</v>
       </c>
       <c r="B27">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C27">
-        <v>5.618000030517578</v>
+        <v>5.220000267028809</v>
       </c>
       <c r="D27">
-        <v>8.022500038146973</v>
+        <v>5.349999904632568</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -775,27 +775,27 @@
         <v>-1.549999952316284</v>
       </c>
       <c r="B28">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C28">
-        <v>0.7499999403953552</v>
+        <v>0.3499999046325684</v>
       </c>
       <c r="D28">
-        <v>1.93749988079071</v>
+        <v>1.291666626930237</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29">
-        <v>-7.938000202178955</v>
+        <v>-7.940000057220459</v>
       </c>
       <c r="B29">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C29">
-        <v>7.138000011444092</v>
+        <v>6.739999771118164</v>
       </c>
       <c r="D29">
-        <v>9.922499656677246</v>
+        <v>6.616666316986084</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -814,13 +814,13 @@
     </row>
     <row r="31" spans="1:4">
       <c r="A31">
-        <v>-9.515999794006348</v>
+        <v>-9.520000457763672</v>
       </c>
       <c r="B31">
         <v>0</v>
       </c>
       <c r="C31">
-        <v>9.515999794006348</v>
+        <v>9.520000457763672</v>
       </c>
       <c r="D31" t="s">
         <v>4</v>
@@ -845,24 +845,24 @@
         <v>-7.070000171661377</v>
       </c>
       <c r="B33">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C33">
-        <v>6.269999980926514</v>
+        <v>5.869999885559082</v>
       </c>
       <c r="D33">
-        <v>8.837499618530273</v>
+        <v>5.891666412353516</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34">
-        <v>-3.270999908447266</v>
+        <v>-3.269999980926514</v>
       </c>
       <c r="B34">
         <v>0</v>
       </c>
       <c r="C34">
-        <v>3.270999908447266</v>
+        <v>3.269999980926514</v>
       </c>
       <c r="D34" t="s">
         <v>4</v>
@@ -870,55 +870,55 @@
     </row>
     <row r="35" spans="1:4">
       <c r="A35">
-        <v>-4.973000049591064</v>
+        <v>-4.96999979019165</v>
       </c>
       <c r="B35">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C35">
-        <v>4.172999858856201</v>
+        <v>3.769999742507935</v>
       </c>
       <c r="D35">
-        <v>6.216249942779541</v>
+        <v>4.141666412353516</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36">
-        <v>-5.061999797821045</v>
+        <v>-5.059999942779541</v>
       </c>
       <c r="B36">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C36">
-        <v>4.261999607086182</v>
+        <v>3.859999895095825</v>
       </c>
       <c r="D36">
-        <v>6.327499866485596</v>
+        <v>4.216666221618652</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37">
-        <v>-7.198999881744385</v>
+        <v>-7.199999809265137</v>
       </c>
       <c r="B37">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C37">
-        <v>6.398999691009521</v>
+        <v>6</v>
       </c>
       <c r="D37">
-        <v>8.998749732971191</v>
+        <v>5.999999523162842</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38">
-        <v>-7.27299976348877</v>
+        <v>-7.269999980926514</v>
       </c>
       <c r="B38">
         <v>0</v>
       </c>
       <c r="C38">
-        <v>7.27299976348877</v>
+        <v>7.269999980926514</v>
       </c>
       <c r="D38" t="s">
         <v>4</v>
@@ -926,27 +926,27 @@
     </row>
     <row r="39" spans="1:4">
       <c r="A39">
-        <v>-8.086000442504883</v>
+        <v>-8.090000152587891</v>
       </c>
       <c r="B39">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C39">
-        <v>7.28600025177002</v>
+        <v>6.890000343322754</v>
       </c>
       <c r="D39">
-        <v>10.10750007629395</v>
+        <v>6.741666316986084</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40">
-        <v>-8.633000373840332</v>
+        <v>-8.630000114440918</v>
       </c>
       <c r="B40">
         <v>0</v>
       </c>
       <c r="C40">
-        <v>8.633000373840332</v>
+        <v>8.630000114440918</v>
       </c>
       <c r="D40" t="s">
         <v>4</v>
@@ -954,27 +954,27 @@
     </row>
     <row r="41" spans="1:4">
       <c r="A41">
-        <v>-7.065999984741211</v>
+        <v>-7.070000171661377</v>
       </c>
       <c r="B41">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C41">
-        <v>6.265999794006348</v>
+        <v>5.869999885559082</v>
       </c>
       <c r="D41">
-        <v>8.832499504089355</v>
+        <v>5.891666412353516</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42">
-        <v>-3.687999963760376</v>
+        <v>-3.690000057220459</v>
       </c>
       <c r="B42">
         <v>0</v>
       </c>
       <c r="C42">
-        <v>3.687999963760376</v>
+        <v>3.690000057220459</v>
       </c>
       <c r="D42" t="s">
         <v>4</v>
@@ -985,24 +985,24 @@
         <v>-11.5</v>
       </c>
       <c r="B43">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C43">
-        <v>10.69999980926514</v>
+        <v>10.30000019073486</v>
       </c>
       <c r="D43">
-        <v>14.375</v>
+        <v>9.583333015441895</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44">
-        <v>-4.526999950408936</v>
+        <v>-4.53000020980835</v>
       </c>
       <c r="B44">
         <v>0</v>
       </c>
       <c r="C44">
-        <v>4.526999950408936</v>
+        <v>4.53000020980835</v>
       </c>
       <c r="D44" t="s">
         <v>4</v>
@@ -1013,52 +1013,52 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B45">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C45">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46">
-        <v>-5.953000068664551</v>
+        <v>-5.949999809265137</v>
       </c>
       <c r="B46">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C46">
-        <v>5.152999877929688</v>
+        <v>4.75</v>
       </c>
       <c r="D46">
-        <v>7.441249847412109</v>
+        <v>4.958333015441895</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47">
-        <v>-7.61299991607666</v>
+        <v>-7.610000133514404</v>
       </c>
       <c r="B47">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C47">
-        <v>6.812999725341797</v>
+        <v>6.409999847412109</v>
       </c>
       <c r="D47">
-        <v>9.516249656677246</v>
+        <v>6.341666698455811</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48">
-        <v>-7.331999778747559</v>
+        <v>-7.329999923706055</v>
       </c>
       <c r="B48">
         <v>0</v>
       </c>
       <c r="C48">
-        <v>7.331999778747559</v>
+        <v>7.329999923706055</v>
       </c>
       <c r="D48" t="s">
         <v>4</v>
@@ -1066,13 +1066,13 @@
     </row>
     <row r="49" spans="1:4">
       <c r="A49">
-        <v>-1.447999954223633</v>
+        <v>-1.450000047683716</v>
       </c>
       <c r="B49">
         <v>0</v>
       </c>
       <c r="C49">
-        <v>1.447999954223633</v>
+        <v>1.450000047683716</v>
       </c>
       <c r="D49" t="s">
         <v>4</v>
@@ -1080,55 +1080,55 @@
     </row>
     <row r="50" spans="1:4">
       <c r="A50">
-        <v>-3.934000015258789</v>
+        <v>-3.930000066757202</v>
       </c>
       <c r="B50">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C50">
-        <v>3.134000062942505</v>
+        <v>2.730000019073486</v>
       </c>
       <c r="D50">
-        <v>4.917500019073486</v>
+        <v>3.274999856948853</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51">
-        <v>-6.10200023651123</v>
+        <v>-6.099999904632568</v>
       </c>
       <c r="B51">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C51">
-        <v>5.302000045776367</v>
+        <v>4.899999618530273</v>
       </c>
       <c r="D51">
-        <v>7.627500057220459</v>
+        <v>5.083333015441895</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52">
-        <v>-8.796999931335449</v>
+        <v>-8.800000190734863</v>
       </c>
       <c r="B52">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C52">
-        <v>7.996999740600586</v>
+        <v>7.600000381469727</v>
       </c>
       <c r="D52">
-        <v>10.99625015258789</v>
+        <v>7.333333015441895</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53">
-        <v>-3.217000007629395</v>
+        <v>-3.220000028610229</v>
       </c>
       <c r="B53">
         <v>0</v>
       </c>
       <c r="C53">
-        <v>3.217000007629395</v>
+        <v>3.220000028610229</v>
       </c>
       <c r="D53" t="s">
         <v>4</v>
@@ -1136,16 +1136,16 @@
     </row>
     <row r="54" spans="1:4">
       <c r="A54">
-        <v>-3.378999948501587</v>
+        <v>-3.380000114440918</v>
       </c>
       <c r="B54">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C54">
-        <v>2.578999996185303</v>
+        <v>2.180000066757202</v>
       </c>
       <c r="D54">
-        <v>4.22374963760376</v>
+        <v>2.816666603088379</v>
       </c>
     </row>
     <row r="55" spans="1:4">
@@ -1153,13 +1153,13 @@
         <v>-4.019999980926514</v>
       </c>
       <c r="B55">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C55">
-        <v>3.220000028610229</v>
+        <v>2.819999933242798</v>
       </c>
       <c r="D55">
-        <v>5.025000095367432</v>
+        <v>3.349999904632568</v>
       </c>
     </row>
     <row r="56" spans="1:4">
@@ -1167,52 +1167,52 @@
         <v>-3.410000085830688</v>
       </c>
       <c r="B56">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C56">
-        <v>2.610000133514404</v>
+        <v>2.210000038146973</v>
       </c>
       <c r="D56">
-        <v>4.262499809265137</v>
+        <v>2.841666698455811</v>
       </c>
     </row>
     <row r="57" spans="1:4">
       <c r="A57">
-        <v>-1.835000038146973</v>
+        <v>-1.830000042915344</v>
       </c>
       <c r="B57">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C57">
-        <v>1.035000085830688</v>
+        <v>0.6299999952316284</v>
       </c>
       <c r="D57">
-        <v>2.293750047683716</v>
+        <v>1.524999976158142</v>
       </c>
     </row>
     <row r="58" spans="1:4">
       <c r="A58">
-        <v>-7.695000171661377</v>
+        <v>-7.699999809265137</v>
       </c>
       <c r="B58">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C58">
-        <v>6.894999980926514</v>
+        <v>6.5</v>
       </c>
       <c r="D58">
-        <v>9.618749618530273</v>
+        <v>6.416666030883789</v>
       </c>
     </row>
     <row r="59" spans="1:4">
       <c r="A59">
-        <v>-1.447999954223633</v>
+        <v>-1.450000047683716</v>
       </c>
       <c r="B59">
         <v>0</v>
       </c>
       <c r="C59">
-        <v>1.447999954223633</v>
+        <v>1.450000047683716</v>
       </c>
       <c r="D59" t="s">
         <v>4</v>
@@ -1220,30 +1220,30 @@
     </row>
     <row r="60" spans="1:4">
       <c r="A60">
-        <v>-1.935999989509583</v>
+        <v>-1.940000057220459</v>
       </c>
       <c r="B60">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C60">
-        <v>1.135999917984009</v>
+        <v>0.7400000095367432</v>
       </c>
       <c r="D60">
-        <v>2.419999837875366</v>
+        <v>1.616666674613953</v>
       </c>
     </row>
     <row r="61" spans="1:4">
       <c r="A61">
-        <v>-3.351999998092651</v>
+        <v>-3.349999904632568</v>
       </c>
       <c r="B61">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C61">
-        <v>2.552000045776367</v>
+        <v>2.149999856948853</v>
       </c>
       <c r="D61">
-        <v>4.190000057220459</v>
+        <v>2.791666507720947</v>
       </c>
     </row>
     <row r="62" spans="1:4">
@@ -1251,24 +1251,24 @@
         <v>-8.680000305175781</v>
       </c>
       <c r="B62">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C62">
-        <v>7.880000114440918</v>
+        <v>7.480000495910645</v>
       </c>
       <c r="D62">
-        <v>10.85000038146973</v>
+        <v>7.233333110809326</v>
       </c>
     </row>
     <row r="63" spans="1:4">
       <c r="A63">
-        <v>-3.844000101089478</v>
+        <v>-3.839999914169312</v>
       </c>
       <c r="B63">
         <v>0</v>
       </c>
       <c r="C63">
-        <v>3.844000101089478</v>
+        <v>3.839999914169312</v>
       </c>
       <c r="D63" t="s">
         <v>4</v>
@@ -1276,30 +1276,30 @@
     </row>
     <row r="64" spans="1:4">
       <c r="A64">
-        <v>-1.58899998664856</v>
+        <v>-1.590000033378601</v>
       </c>
       <c r="B64">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C64">
-        <v>0.7889999747276306</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="D64">
-        <v>1.986249923706055</v>
+        <v>1.324999928474426</v>
       </c>
     </row>
     <row r="65" spans="1:4">
       <c r="A65">
-        <v>-3.891000032424927</v>
+        <v>-3.890000104904175</v>
       </c>
       <c r="B65">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C65">
-        <v>3.091000080108643</v>
+        <v>2.690000057220459</v>
       </c>
       <c r="D65">
-        <v>4.863749980926514</v>
+        <v>3.241666555404663</v>
       </c>
     </row>
     <row r="66" spans="1:4">
@@ -1307,38 +1307,38 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B66">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C66">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D66">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:4">
       <c r="A67">
-        <v>-8.211000442504883</v>
+        <v>-8.210000038146973</v>
       </c>
       <c r="B67">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C67">
-        <v>7.41100025177002</v>
+        <v>7.010000228881836</v>
       </c>
       <c r="D67">
-        <v>10.26375007629395</v>
+        <v>6.841666221618652</v>
       </c>
     </row>
     <row r="68" spans="1:4">
       <c r="A68">
-        <v>-1.199000000953674</v>
+        <v>-1.200000047683716</v>
       </c>
       <c r="B68">
         <v>0</v>
       </c>
       <c r="C68">
-        <v>1.199000000953674</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="D68" t="s">
         <v>4</v>
@@ -1346,27 +1346,27 @@
     </row>
     <row r="69" spans="1:4">
       <c r="A69">
-        <v>-10.66399955749512</v>
+        <v>-10.65999984741211</v>
       </c>
       <c r="B69">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C69">
-        <v>9.863999366760254</v>
+        <v>9.460000038146973</v>
       </c>
       <c r="D69">
-        <v>13.32999897003174</v>
+        <v>8.883333206176758</v>
       </c>
     </row>
     <row r="70" spans="1:4">
       <c r="A70">
-        <v>-14.13300037384033</v>
+        <v>-14.13000011444092</v>
       </c>
       <c r="B70">
         <v>0</v>
       </c>
       <c r="C70">
-        <v>14.13300037384033</v>
+        <v>14.13000011444092</v>
       </c>
       <c r="D70" t="s">
         <v>4</v>
@@ -1374,13 +1374,13 @@
     </row>
     <row r="71" spans="1:4">
       <c r="A71">
-        <v>-8.22700023651123</v>
+        <v>-8.229999542236328</v>
       </c>
       <c r="B71">
         <v>0</v>
       </c>
       <c r="C71">
-        <v>8.22700023651123</v>
+        <v>8.229999542236328</v>
       </c>
       <c r="D71" t="s">
         <v>4</v>
@@ -1402,41 +1402,41 @@
     </row>
     <row r="73" spans="1:4">
       <c r="A73">
-        <v>-1.447999954223633</v>
+        <v>-1.450000047683716</v>
       </c>
       <c r="B73">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C73">
-        <v>0.6479999423027039</v>
+        <v>0.25</v>
       </c>
       <c r="D73">
-        <v>1.809999942779541</v>
+        <v>1.208333373069763</v>
       </c>
     </row>
     <row r="74" spans="1:4">
       <c r="A74">
-        <v>-7.218999862670898</v>
+        <v>-7.21999979019165</v>
       </c>
       <c r="B74">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C74">
-        <v>6.418999671936035</v>
+        <v>6.019999504089355</v>
       </c>
       <c r="D74">
-        <v>9.023749351501465</v>
+        <v>6.016666412353516</v>
       </c>
     </row>
     <row r="75" spans="1:4">
       <c r="A75">
-        <v>-9.078000068664551</v>
+        <v>-9.079999923706055</v>
       </c>
       <c r="B75">
         <v>0</v>
       </c>
       <c r="C75">
-        <v>9.078000068664551</v>
+        <v>9.079999923706055</v>
       </c>
       <c r="D75" t="s">
         <v>4</v>
@@ -1444,13 +1444,13 @@
     </row>
     <row r="76" spans="1:4">
       <c r="A76">
-        <v>-6.945000171661377</v>
+        <v>-6.949999809265137</v>
       </c>
       <c r="B76">
         <v>0</v>
       </c>
       <c r="C76">
-        <v>6.945000171661377</v>
+        <v>6.949999809265137</v>
       </c>
       <c r="D76" t="s">
         <v>4</v>
@@ -1458,13 +1458,13 @@
     </row>
     <row r="77" spans="1:4">
       <c r="A77">
-        <v>-3.065999984741211</v>
+        <v>-3.069999933242798</v>
       </c>
       <c r="B77">
         <v>0</v>
       </c>
       <c r="C77">
-        <v>3.065999984741211</v>
+        <v>3.069999933242798</v>
       </c>
       <c r="D77" t="s">
         <v>4</v>
@@ -1472,139 +1472,139 @@
     </row>
     <row r="78" spans="1:4">
       <c r="A78">
-        <v>-4.438000202178955</v>
+        <v>-4.440000057220459</v>
       </c>
       <c r="B78">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C78">
-        <v>3.638000249862671</v>
+        <v>3.240000009536743</v>
       </c>
       <c r="D78">
-        <v>5.547500133514404</v>
+        <v>3.699999809265137</v>
       </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79">
-        <v>-2.181999921798706</v>
+        <v>-2.180000066757202</v>
       </c>
       <c r="B79">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C79">
-        <v>1.381999969482422</v>
+        <v>0.9800000190734863</v>
       </c>
       <c r="D79">
-        <v>2.727499961853027</v>
+        <v>1.816666603088379</v>
       </c>
     </row>
     <row r="80" spans="1:4">
       <c r="A80">
-        <v>-3.454999923706055</v>
+        <v>-3.460000038146973</v>
       </c>
       <c r="B80">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C80">
-        <v>2.654999971389771</v>
+        <v>2.259999990463257</v>
       </c>
       <c r="D80">
-        <v>4.318749904632568</v>
+        <v>2.883333206176758</v>
       </c>
     </row>
     <row r="81" spans="1:4">
       <c r="A81">
-        <v>-1.935999989509583</v>
+        <v>-1.940000057220459</v>
       </c>
       <c r="B81">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C81">
-        <v>1.135999917984009</v>
+        <v>0.7400000095367432</v>
       </c>
       <c r="D81">
-        <v>2.419999837875366</v>
+        <v>1.616666674613953</v>
       </c>
     </row>
     <row r="82" spans="1:4">
       <c r="A82">
-        <v>-2.181999921798706</v>
+        <v>-2.180000066757202</v>
       </c>
       <c r="B82">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C82">
-        <v>1.381999969482422</v>
+        <v>0.9800000190734863</v>
       </c>
       <c r="D82">
-        <v>2.727499961853027</v>
+        <v>1.816666603088379</v>
       </c>
     </row>
     <row r="83" spans="1:4">
       <c r="A83">
-        <v>-5.843999862670898</v>
+        <v>-5.840000152587891</v>
       </c>
       <c r="B83">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C83">
-        <v>5.043999671936035</v>
+        <v>4.640000343322754</v>
       </c>
       <c r="D83">
-        <v>7.304999828338623</v>
+        <v>4.866666793823242</v>
       </c>
     </row>
     <row r="84" spans="1:4">
       <c r="A84">
-        <v>-2.082000017166138</v>
+        <v>-2.079999923706055</v>
       </c>
       <c r="B84">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C84">
-        <v>1.282000064849854</v>
+        <v>0.8799998760223389</v>
       </c>
       <c r="D84">
-        <v>2.602499961853027</v>
+        <v>1.733333230018616</v>
       </c>
     </row>
     <row r="85" spans="1:4">
       <c r="A85">
-        <v>-2.181999921798706</v>
+        <v>-2.180000066757202</v>
       </c>
       <c r="B85">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C85">
-        <v>1.381999969482422</v>
+        <v>0.9800000190734863</v>
       </c>
       <c r="D85">
-        <v>2.727499961853027</v>
+        <v>1.816666603088379</v>
       </c>
     </row>
     <row r="86" spans="1:4">
       <c r="A86">
-        <v>-8.991999626159668</v>
+        <v>-8.989999771118164</v>
       </c>
       <c r="B86">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C86">
-        <v>8.191999435424805</v>
+        <v>7.789999961853027</v>
       </c>
       <c r="D86">
-        <v>11.23999977111816</v>
+        <v>7.491666316986084</v>
       </c>
     </row>
     <row r="87" spans="1:4">
       <c r="A87">
-        <v>-6.781000137329102</v>
+        <v>-6.78000020980835</v>
       </c>
       <c r="B87">
         <v>0</v>
       </c>
       <c r="C87">
-        <v>6.781000137329102</v>
+        <v>6.78000020980835</v>
       </c>
       <c r="D87" t="s">
         <v>4</v>
@@ -1612,184 +1612,184 @@
     </row>
     <row r="88" spans="1:4">
       <c r="A88">
-        <v>-3.065999984741211</v>
+        <v>-3.069999933242798</v>
       </c>
       <c r="B88">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C88">
-        <v>2.266000032424927</v>
+        <v>1.869999885559082</v>
       </c>
       <c r="D88">
-        <v>3.832499980926514</v>
+        <v>2.558333158493042</v>
       </c>
     </row>
     <row r="89" spans="1:4">
       <c r="A89">
-        <v>-1.935999989509583</v>
+        <v>-1.940000057220459</v>
       </c>
       <c r="B89">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C89">
-        <v>1.135999917984009</v>
+        <v>0.7400000095367432</v>
       </c>
       <c r="D89">
-        <v>2.419999837875366</v>
+        <v>1.616666674613953</v>
       </c>
     </row>
     <row r="90" spans="1:4">
       <c r="A90">
-        <v>-4.390999794006348</v>
+        <v>-4.389999866485596</v>
       </c>
       <c r="B90">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C90">
-        <v>3.590999841690063</v>
+        <v>3.18999981880188</v>
       </c>
       <c r="D90">
-        <v>5.488749504089355</v>
+        <v>3.65833306312561</v>
       </c>
     </row>
     <row r="91" spans="1:4">
       <c r="A91">
-        <v>-1.935999989509583</v>
+        <v>-1.940000057220459</v>
       </c>
       <c r="B91">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C91">
-        <v>1.135999917984009</v>
+        <v>0.7400000095367432</v>
       </c>
       <c r="D91">
-        <v>2.419999837875366</v>
+        <v>1.616666674613953</v>
       </c>
     </row>
     <row r="92" spans="1:4">
       <c r="A92">
-        <v>-1.835000038146973</v>
+        <v>-1.830000042915344</v>
       </c>
       <c r="B92">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C92">
-        <v>1.035000085830688</v>
+        <v>0.6299999952316284</v>
       </c>
       <c r="D92">
-        <v>2.293750047683716</v>
+        <v>1.524999976158142</v>
       </c>
     </row>
     <row r="93" spans="1:4">
       <c r="A93">
-        <v>-2.332000017166138</v>
+        <v>-2.329999923706055</v>
       </c>
       <c r="B93">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C93">
-        <v>1.532000064849854</v>
+        <v>1.129999876022339</v>
       </c>
       <c r="D93">
-        <v>2.914999961853027</v>
+        <v>1.941666483879089</v>
       </c>
     </row>
     <row r="94" spans="1:4">
       <c r="A94">
-        <v>-2.437999963760376</v>
+        <v>-2.440000057220459</v>
       </c>
       <c r="B94">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C94">
-        <v>1.638000011444092</v>
+        <v>1.240000009536743</v>
       </c>
       <c r="D94">
-        <v>3.047499895095825</v>
+        <v>2.033333301544189</v>
       </c>
     </row>
     <row r="95" spans="1:4">
       <c r="A95">
-        <v>-4.668000221252441</v>
+        <v>-4.670000076293945</v>
       </c>
       <c r="B95">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C95">
-        <v>3.868000268936157</v>
+        <v>3.470000028610229</v>
       </c>
       <c r="D95">
-        <v>5.835000038146973</v>
+        <v>3.891666650772095</v>
       </c>
     </row>
     <row r="96" spans="1:4">
       <c r="A96">
-        <v>-3.844000101089478</v>
+        <v>-3.839999914169312</v>
       </c>
       <c r="B96">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C96">
-        <v>3.044000148773193</v>
+        <v>2.639999866485596</v>
       </c>
       <c r="D96">
-        <v>4.804999828338623</v>
+        <v>3.199999809265137</v>
       </c>
     </row>
     <row r="97" spans="1:4">
       <c r="A97">
-        <v>-2.13700008392334</v>
+        <v>-2.140000104904175</v>
       </c>
       <c r="B97">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C97">
-        <v>1.337000131607056</v>
+        <v>0.940000057220459</v>
       </c>
       <c r="D97">
-        <v>2.671250104904175</v>
+        <v>1.783333301544189</v>
       </c>
     </row>
     <row r="98" spans="1:4">
       <c r="A98">
-        <v>-2.496000051498413</v>
+        <v>-2.5</v>
       </c>
       <c r="B98">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C98">
-        <v>1.696000099182129</v>
+        <v>1.299999952316284</v>
       </c>
       <c r="D98">
-        <v>3.120000123977661</v>
+        <v>2.083333253860474</v>
       </c>
     </row>
     <row r="99" spans="1:4">
       <c r="A99">
-        <v>-3.598000049591064</v>
+        <v>-3.599999904632568</v>
       </c>
       <c r="B99">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C99">
-        <v>2.79800009727478</v>
+        <v>2.399999856948853</v>
       </c>
       <c r="D99">
-        <v>4.497499942779541</v>
+        <v>2.999999761581421</v>
       </c>
     </row>
     <row r="100" spans="1:4">
       <c r="A100">
-        <v>-1.58899998664856</v>
+        <v>-1.590000033378601</v>
       </c>
       <c r="B100">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C100">
-        <v>0.7889999747276306</v>
+        <v>0.3899999856948853</v>
       </c>
       <c r="D100">
-        <v>1.986249923706055</v>
+        <v>1.324999928474426</v>
       </c>
     </row>
     <row r="101" spans="1:4">
@@ -1797,41 +1797,41 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B101">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C101">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D101">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102" spans="1:4">
       <c r="A102">
-        <v>-2.427999973297119</v>
+        <v>-2.430000066757202</v>
       </c>
       <c r="B102">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C102">
-        <v>1.628000020980835</v>
+        <v>1.230000019073486</v>
       </c>
       <c r="D102">
-        <v>3.034999847412109</v>
+        <v>2.024999856948853</v>
       </c>
     </row>
     <row r="103" spans="1:4">
       <c r="A103">
-        <v>-1.761000037193298</v>
+        <v>-1.759999990463257</v>
       </c>
       <c r="B103">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C103">
-        <v>0.9610000252723694</v>
+        <v>0.559999942779541</v>
       </c>
       <c r="D103">
-        <v>2.201250076293945</v>
+        <v>1.466666579246521</v>
       </c>
     </row>
     <row r="104" spans="1:4">
@@ -1839,52 +1839,52 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B104">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C104">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D104">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105" spans="1:4">
       <c r="A105">
-        <v>-1.447999954223633</v>
+        <v>-1.450000047683716</v>
       </c>
       <c r="B105">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C105">
-        <v>0.6479999423027039</v>
+        <v>0.25</v>
       </c>
       <c r="D105">
-        <v>1.809999942779541</v>
+        <v>1.208333373069763</v>
       </c>
     </row>
     <row r="106" spans="1:4">
       <c r="A106">
-        <v>-6.632999897003174</v>
+        <v>-6.630000114440918</v>
       </c>
       <c r="B106">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C106">
-        <v>5.832999706268311</v>
+        <v>5.430000305175781</v>
       </c>
       <c r="D106">
-        <v>8.29124927520752</v>
+        <v>5.525000095367432</v>
       </c>
     </row>
     <row r="107" spans="1:4">
       <c r="A107">
-        <v>-4.046999931335449</v>
+        <v>-4.050000190734863</v>
       </c>
       <c r="B107">
         <v>0</v>
       </c>
       <c r="C107">
-        <v>4.046999931335449</v>
+        <v>4.050000190734863</v>
       </c>
       <c r="D107" t="s">
         <v>4</v>
@@ -1892,30 +1892,30 @@
     </row>
     <row r="108" spans="1:4">
       <c r="A108">
-        <v>-3.555000066757202</v>
+        <v>-3.549999952316284</v>
       </c>
       <c r="B108">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C108">
-        <v>2.755000114440918</v>
+        <v>2.349999904632568</v>
       </c>
       <c r="D108">
-        <v>4.443749904632568</v>
+        <v>2.958333253860474</v>
       </c>
     </row>
     <row r="109" spans="1:4">
       <c r="A109">
-        <v>-2.517999887466431</v>
+        <v>-2.519999980926514</v>
       </c>
       <c r="B109">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C109">
-        <v>1.717999935150146</v>
+        <v>1.319999933242798</v>
       </c>
       <c r="D109">
-        <v>3.147499799728394</v>
+        <v>2.099999904632568</v>
       </c>
     </row>
     <row r="110" spans="1:4">
@@ -1923,55 +1923,55 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B110">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C110">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D110">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111" spans="1:4">
       <c r="A111">
-        <v>-1.447999954223633</v>
+        <v>-1.450000047683716</v>
       </c>
       <c r="B111">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C111">
-        <v>0.6479999423027039</v>
+        <v>0.25</v>
       </c>
       <c r="D111">
-        <v>1.809999942779541</v>
+        <v>1.208333373069763</v>
       </c>
     </row>
     <row r="112" spans="1:4">
       <c r="A112">
-        <v>-3.167999982833862</v>
+        <v>-3.170000076293945</v>
       </c>
       <c r="B112">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C112">
-        <v>2.368000030517578</v>
+        <v>1.970000028610229</v>
       </c>
       <c r="D112">
-        <v>3.960000038146973</v>
+        <v>2.641666650772095</v>
       </c>
     </row>
     <row r="113" spans="1:4">
       <c r="A113">
-        <v>-1.935999989509583</v>
+        <v>-1.940000057220459</v>
       </c>
       <c r="B113">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C113">
-        <v>1.135999917984009</v>
+        <v>0.7400000095367432</v>
       </c>
       <c r="D113">
-        <v>2.419999837875366</v>
+        <v>1.616666674613953</v>
       </c>
     </row>
     <row r="114" spans="1:4">
@@ -1979,13 +1979,13 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B114">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C114">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D114">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="115" spans="1:4">
@@ -1993,41 +1993,41 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B115">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C115">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D115">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="116" spans="1:4">
       <c r="A116">
-        <v>-1.935999989509583</v>
+        <v>-1.940000057220459</v>
       </c>
       <c r="B116">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C116">
-        <v>1.135999917984009</v>
+        <v>0.7400000095367432</v>
       </c>
       <c r="D116">
-        <v>2.419999837875366</v>
+        <v>1.616666674613953</v>
       </c>
     </row>
     <row r="117" spans="1:4">
       <c r="A117">
-        <v>-1.835000038146973</v>
+        <v>-1.830000042915344</v>
       </c>
       <c r="B117">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C117">
-        <v>1.035000085830688</v>
+        <v>0.6299999952316284</v>
       </c>
       <c r="D117">
-        <v>2.293750047683716</v>
+        <v>1.524999976158142</v>
       </c>
     </row>
     <row r="118" spans="1:4">
@@ -2035,13 +2035,13 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B118">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C118">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D118">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119" spans="1:4">
@@ -2049,27 +2049,27 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B119">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C119">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D119">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="120" spans="1:4">
       <c r="A120">
-        <v>-2.427999973297119</v>
+        <v>-2.430000066757202</v>
       </c>
       <c r="B120">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C120">
-        <v>1.628000020980835</v>
+        <v>1.230000019073486</v>
       </c>
       <c r="D120">
-        <v>3.034999847412109</v>
+        <v>2.024999856948853</v>
       </c>
     </row>
     <row r="121" spans="1:4">
@@ -2077,27 +2077,27 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B121">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C121">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D121">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="122" spans="1:4">
       <c r="A122">
-        <v>-1.199000000953674</v>
+        <v>-1.200000047683716</v>
       </c>
       <c r="B122">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C122">
-        <v>0.3989999890327454</v>
+        <v>0</v>
       </c>
       <c r="D122">
-        <v>1.498749971389771</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123" spans="1:4">
@@ -2105,13 +2105,13 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B123">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C123">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D123">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124" spans="1:4">
@@ -2119,41 +2119,41 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B124">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C124">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D124">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="125" spans="1:4">
       <c r="A125">
-        <v>-3.164000034332275</v>
+        <v>-3.160000085830688</v>
       </c>
       <c r="B125">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C125">
-        <v>2.364000082015991</v>
+        <v>1.960000038146973</v>
       </c>
       <c r="D125">
-        <v>3.954999923706055</v>
+        <v>2.633333206176758</v>
       </c>
     </row>
     <row r="126" spans="1:4">
       <c r="A126">
-        <v>-2.437999963760376</v>
+        <v>-2.440000057220459</v>
       </c>
       <c r="B126">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C126">
-        <v>1.638000011444092</v>
+        <v>1.240000009536743</v>
       </c>
       <c r="D126">
-        <v>3.047499895095825</v>
+        <v>2.033333301544189</v>
       </c>
     </row>
     <row r="127" spans="1:4">
@@ -2161,13 +2161,13 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B127">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C127">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D127">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="128" spans="1:4">
@@ -2175,27 +2175,27 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B128">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C128">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D128">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="129" spans="1:4">
       <c r="A129">
-        <v>-2.115000009536743</v>
+        <v>-2.119999885559082</v>
       </c>
       <c r="B129">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C129">
-        <v>1.315000057220459</v>
+        <v>0.9199998378753662</v>
       </c>
       <c r="D129">
-        <v>2.643749952316284</v>
+        <v>1.766666531562805</v>
       </c>
     </row>
     <row r="130" spans="1:4">
@@ -2203,27 +2203,27 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B130">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C130">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D130">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131" spans="1:4">
       <c r="A131">
-        <v>-1.935999989509583</v>
+        <v>-1.940000057220459</v>
       </c>
       <c r="B131">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C131">
-        <v>1.135999917984009</v>
+        <v>0.7400000095367432</v>
       </c>
       <c r="D131">
-        <v>2.419999837875366</v>
+        <v>1.616666674613953</v>
       </c>
     </row>
     <row r="132" spans="1:4">
@@ -2231,13 +2231,13 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B132">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C132">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D132">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="133" spans="1:4">
@@ -2245,111 +2245,111 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B133">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C133">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D133">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134" spans="1:4">
       <c r="A134">
-        <v>-3.164000034332275</v>
+        <v>-3.160000085830688</v>
       </c>
       <c r="B134">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C134">
-        <v>2.364000082015991</v>
+        <v>1.960000038146973</v>
       </c>
       <c r="D134">
-        <v>3.954999923706055</v>
+        <v>2.633333206176758</v>
       </c>
     </row>
     <row r="135" spans="1:4">
       <c r="A135">
-        <v>-2.427999973297119</v>
+        <v>-2.430000066757202</v>
       </c>
       <c r="B135">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C135">
-        <v>1.628000020980835</v>
+        <v>1.230000019073486</v>
       </c>
       <c r="D135">
-        <v>3.034999847412109</v>
+        <v>2.024999856948853</v>
       </c>
     </row>
     <row r="136" spans="1:4">
       <c r="A136">
-        <v>-2.181999921798706</v>
+        <v>-2.180000066757202</v>
       </c>
       <c r="B136">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C136">
-        <v>1.381999969482422</v>
+        <v>0.9800000190734863</v>
       </c>
       <c r="D136">
-        <v>2.727499961853027</v>
+        <v>1.816666603088379</v>
       </c>
     </row>
     <row r="137" spans="1:4">
       <c r="A137">
-        <v>-1.199000000953674</v>
+        <v>-1.200000047683716</v>
       </c>
       <c r="B137">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C137">
-        <v>0.3989999890327454</v>
+        <v>0</v>
       </c>
       <c r="D137">
-        <v>1.498749971389771</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138" spans="1:4">
       <c r="A138">
-        <v>-1.835000038146973</v>
+        <v>-1.830000042915344</v>
       </c>
       <c r="B138">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C138">
-        <v>1.035000085830688</v>
+        <v>0.6299999952316284</v>
       </c>
       <c r="D138">
-        <v>2.293750047683716</v>
+        <v>1.524999976158142</v>
       </c>
     </row>
     <row r="139" spans="1:4">
       <c r="A139">
-        <v>-2.073999881744385</v>
+        <v>-2.069999933242798</v>
       </c>
       <c r="B139">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C139">
-        <v>1.273999929428101</v>
+        <v>0.869999885559082</v>
       </c>
       <c r="D139">
-        <v>2.592499732971191</v>
+        <v>1.724999904632568</v>
       </c>
     </row>
     <row r="140" spans="1:4">
       <c r="A140">
-        <v>-1.935999989509583</v>
+        <v>-1.940000057220459</v>
       </c>
       <c r="B140">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C140">
-        <v>1.135999917984009</v>
+        <v>0.7400000095367432</v>
       </c>
       <c r="D140">
-        <v>2.419999837875366</v>
+        <v>1.616666674613953</v>
       </c>
     </row>
     <row r="141" spans="1:4">
@@ -2357,27 +2357,27 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B141">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C141">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D141">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="142" spans="1:4">
       <c r="A142">
-        <v>-1.447999954223633</v>
+        <v>-1.450000047683716</v>
       </c>
       <c r="B142">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C142">
-        <v>0.6479999423027039</v>
+        <v>0.25</v>
       </c>
       <c r="D142">
-        <v>1.809999942779541</v>
+        <v>1.208333373069763</v>
       </c>
     </row>
     <row r="143" spans="1:4">
@@ -2385,13 +2385,13 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B143">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C143">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D143">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="144" spans="1:4">
@@ -2399,13 +2399,13 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B144">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C144">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D144">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="145" spans="1:4">
@@ -2413,13 +2413,13 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B145">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C145">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D145">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="146" spans="1:4">
@@ -2427,13 +2427,13 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B146">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C146">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D146">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="147" spans="1:4">
@@ -2441,13 +2441,13 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B147">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C147">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D147">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="148" spans="1:4">
@@ -2455,122 +2455,122 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B148">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C148">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D148">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="149" spans="1:4">
       <c r="A149">
-        <v>-3.252000093460083</v>
+        <v>-3.25</v>
       </c>
       <c r="B149">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C149">
-        <v>2.452000141143799</v>
+        <v>2.049999952316284</v>
       </c>
       <c r="D149">
-        <v>4.065000057220459</v>
+        <v>2.708333253860474</v>
       </c>
     </row>
     <row r="150" spans="1:4">
       <c r="A150">
-        <v>-1.447999954223633</v>
+        <v>-1.450000047683716</v>
       </c>
       <c r="B150">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C150">
-        <v>0.6479999423027039</v>
+        <v>0.25</v>
       </c>
       <c r="D150">
-        <v>1.809999942779541</v>
+        <v>1.208333373069763</v>
       </c>
     </row>
     <row r="151" spans="1:4">
       <c r="A151">
-        <v>-4.671999931335449</v>
+        <v>-4.670000076293945</v>
       </c>
       <c r="B151">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C151">
-        <v>3.871999979019165</v>
+        <v>3.470000028610229</v>
       </c>
       <c r="D151">
-        <v>5.839999675750732</v>
+        <v>3.891666650772095</v>
       </c>
     </row>
     <row r="152" spans="1:4">
       <c r="A152">
-        <v>-1.935999989509583</v>
+        <v>-1.940000057220459</v>
       </c>
       <c r="B152">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C152">
-        <v>1.135999917984009</v>
+        <v>0.7400000095367432</v>
       </c>
       <c r="D152">
-        <v>2.419999837875366</v>
+        <v>1.616666674613953</v>
       </c>
     </row>
     <row r="153" spans="1:4">
       <c r="A153">
-        <v>-1.447999954223633</v>
+        <v>-1.450000047683716</v>
       </c>
       <c r="B153">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C153">
-        <v>0.6479999423027039</v>
+        <v>0.25</v>
       </c>
       <c r="D153">
-        <v>1.809999942779541</v>
+        <v>1.208333373069763</v>
       </c>
     </row>
     <row r="154" spans="1:4">
       <c r="A154">
-        <v>-1.935999989509583</v>
+        <v>-1.940000057220459</v>
       </c>
       <c r="B154">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C154">
-        <v>1.135999917984009</v>
+        <v>0.7400000095367432</v>
       </c>
       <c r="D154">
-        <v>2.419999837875366</v>
+        <v>1.616666674613953</v>
       </c>
     </row>
     <row r="155" spans="1:4">
       <c r="A155">
-        <v>-5.742000102996826</v>
+        <v>-5.739999771118164</v>
       </c>
       <c r="B155">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C155">
-        <v>4.941999912261963</v>
+        <v>4.539999961853027</v>
       </c>
       <c r="D155">
-        <v>7.177500247955322</v>
+        <v>4.783332824707031</v>
       </c>
     </row>
     <row r="156" spans="1:4">
       <c r="A156">
-        <v>-2.86299991607666</v>
+        <v>-2.859999895095825</v>
       </c>
       <c r="B156">
         <v>0</v>
       </c>
       <c r="C156">
-        <v>2.86299991607666</v>
+        <v>2.859999895095825</v>
       </c>
       <c r="D156" t="s">
         <v>4</v>
@@ -2578,16 +2578,16 @@
     </row>
     <row r="157" spans="1:4">
       <c r="A157">
-        <v>-2.023000001907349</v>
+        <v>-2.019999980926514</v>
       </c>
       <c r="B157">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C157">
-        <v>1.223000049591064</v>
+        <v>0.8199999332427979</v>
       </c>
       <c r="D157">
-        <v>2.528749942779541</v>
+        <v>1.683333277702332</v>
       </c>
     </row>
     <row r="158" spans="1:4">
@@ -2595,13 +2595,13 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B158">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C158">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D158">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="159" spans="1:4">
@@ -2609,13 +2609,13 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B159">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C159">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D159">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="160" spans="1:4">
@@ -2623,55 +2623,55 @@
         <v>-1.200000047683716</v>
       </c>
       <c r="B160">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C160">
-        <v>0.4000000357627869</v>
+        <v>0</v>
       </c>
       <c r="D160">
-        <v>1.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="161" spans="1:4">
       <c r="A161">
-        <v>-2.181999921798706</v>
+        <v>-2.180000066757202</v>
       </c>
       <c r="B161">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C161">
-        <v>1.381999969482422</v>
+        <v>0.9800000190734863</v>
       </c>
       <c r="D161">
-        <v>2.727499961853027</v>
+        <v>1.816666603088379</v>
       </c>
     </row>
     <row r="162" spans="1:4">
       <c r="A162">
-        <v>-1.835000038146973</v>
+        <v>-1.830000042915344</v>
       </c>
       <c r="B162">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C162">
-        <v>1.035000085830688</v>
+        <v>0.6299999952316284</v>
       </c>
       <c r="D162">
-        <v>2.293750047683716</v>
+        <v>1.524999976158142</v>
       </c>
     </row>
     <row r="163" spans="1:4">
       <c r="A163">
-        <v>-1.935999989509583</v>
+        <v>-1.940000057220459</v>
       </c>
       <c r="B163">
-        <v>0.800000011920929</v>
+        <v>1.200000047683716</v>
       </c>
       <c r="C163">
-        <v>1.135999917984009</v>
+        <v>0.7400000095367432</v>
       </c>
       <c r="D163">
-        <v>2.419999837875366</v>
+        <v>1.616666674613953</v>
       </c>
     </row>
   </sheetData>

</xml_diff>